<commit_message>
New Website Version retests
</commit_message>
<xml_diff>
--- a/Sessie sheet (testcases) - Front-end.xlsx
+++ b/Sessie sheet (testcases) - Front-end.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Casus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CA031D5-3A41-4413-B7EE-DB8883040517}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{383FCE92-64FA-4F44-85B2-131D52491126}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="251">
   <si>
     <t>Session sheet #</t>
   </si>
@@ -941,9 +941,6 @@
     <t>3. zoekfunctie naar hotels in een plaats geeft geen resultaten</t>
   </si>
   <si>
-    <t>Er worden geen hotels getoond.</t>
-  </si>
-  <si>
     <t>Melding "No matches found" wordt getoond</t>
   </si>
   <si>
@@ -956,15 +953,9 @@
     <t>Geen foutmelding wordt getoond, zoekresultaat verschijnt</t>
   </si>
   <si>
-    <t>Geen foutmelding getoond, zoekresultaat verschijnt. Aantal volwassenen is op 1 persoon gezet.</t>
-  </si>
-  <si>
     <t>Zoekresultaten worden weergegeven</t>
   </si>
   <si>
-    <t>De zoekresultaten worden getoond. Het aantal volwassenen wordt automatisch op 1 gezet.</t>
-  </si>
-  <si>
     <t>Kan niet uitgevoerd worden. Het is niet mogelijk om lege velden te hebben, deze worden automatisch gevuld.</t>
   </si>
   <si>
@@ -1013,13 +1004,7 @@
     <t>website laadt</t>
   </si>
   <si>
-    <t>De pagina die laadt na succesvolle inlog is leeg. Bij teruggaan naar homepage blijkt dat user wel is ingelogd (user Johny in rechter bovenhoek), maar accountdetailspagina blijft leeg.</t>
-  </si>
-  <si>
     <t>phptravels.net</t>
-  </si>
-  <si>
-    <t>Alle schermen laden en zijn inzichtelijk, met uitzondering van de schermen zoals al aangegeven bij andere testcases.</t>
   </si>
   <si>
     <t>Beschikbaar, wordt getoond</t>
@@ -1089,13 +1074,25 @@
     <t>Geen bijzonderheden waargenomen.</t>
   </si>
   <si>
-    <t>De accountpagina is blanco</t>
-  </si>
-  <si>
     <t>Foutmelding: Invalid Email or Password</t>
   </si>
   <si>
     <t>Geregistreerd issue #</t>
+  </si>
+  <si>
+    <t>Hotel Grand Plaza Appartments in London wordt getoond</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>kan niet testen, geen inlog backend</t>
+  </si>
+  <si>
+    <t>De zoekresultaten worden getoond. Het aantal volwassenen wordt automatisch op 2 gezet.</t>
+  </si>
+  <si>
+    <t>Geen foutmelding getoond, zoekresultaat verschijnt. Aantal volwassenen is op 2 persoon gezet.</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1372,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1534,78 +1531,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1613,9 +1538,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1627,6 +1549,78 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1693,13 +1687,14 @@
       <sheetName val="TC5"/>
       <sheetName val="TC6"/>
       <sheetName val="TC7"/>
+      <sheetName val="TC8"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="20">
           <cell r="B20" t="str">
-            <v xml:space="preserve">Beschrijving van de bevinding en verwijzing naar de registratie van de bevinding </v>
+            <v>Zie testcase onderaan de pagina.</v>
           </cell>
         </row>
       </sheetData>
@@ -1709,6 +1704,7 @@
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2046,7 +2042,7 @@
     <col min="1" max="1" width="10.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="32.6640625" style="94" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="69" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -2061,11 +2057,11 @@
       <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="68" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
@@ -2075,14 +2071,14 @@
       <c r="B3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="95" t="s">
-        <v>246</v>
+      <c r="C3" s="70" t="s">
+        <v>241</v>
       </c>
       <c r="D3" s="63" t="str">
         <f>[1]TC1!B20</f>
-        <v xml:space="preserve">Beschrijving van de bevinding en verwijzing naar de registratie van de bevinding </v>
-      </c>
-      <c r="E3" s="92"/>
+        <v>Zie testcase onderaan de pagina.</v>
+      </c>
+      <c r="E3" s="67"/>
     </row>
     <row r="4" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -2091,11 +2087,11 @@
       <c r="B4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="96" t="s">
-        <v>247</v>
+      <c r="C4" s="71" t="s">
+        <v>242</v>
       </c>
       <c r="D4" s="63"/>
-      <c r="E4" s="92"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
@@ -2104,11 +2100,11 @@
       <c r="B5" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="96" t="s">
-        <v>247</v>
+      <c r="C5" s="71" t="s">
+        <v>242</v>
       </c>
       <c r="D5" s="63"/>
-      <c r="E5" s="92"/>
+      <c r="E5" s="67"/>
     </row>
     <row r="6" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -2117,11 +2113,11 @@
       <c r="B6" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="95" t="s">
-        <v>246</v>
+      <c r="C6" s="70" t="s">
+        <v>241</v>
       </c>
       <c r="D6" s="63"/>
-      <c r="E6" s="92"/>
+      <c r="E6" s="67"/>
     </row>
     <row r="7" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
@@ -2130,11 +2126,11 @@
       <c r="B7" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="95" t="s">
-        <v>246</v>
+      <c r="C7" s="70" t="s">
+        <v>241</v>
       </c>
       <c r="D7" s="63"/>
-      <c r="E7" s="92"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
@@ -2143,11 +2139,11 @@
       <c r="B8" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="96" t="s">
-        <v>247</v>
+      <c r="C8" s="71" t="s">
+        <v>242</v>
       </c>
       <c r="D8" s="63"/>
-      <c r="E8" s="92"/>
+      <c r="E8" s="67"/>
     </row>
     <row r="9" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
@@ -2156,11 +2152,11 @@
       <c r="B9" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="95" t="s">
-        <v>246</v>
+      <c r="C9" s="70" t="s">
+        <v>241</v>
       </c>
       <c r="D9" s="63"/>
-      <c r="E9" s="92"/>
+      <c r="E9" s="67"/>
     </row>
     <row r="10" spans="1:5" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -2169,11 +2165,11 @@
       <c r="B10" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="96" t="s">
-        <v>247</v>
+      <c r="C10" s="71" t="s">
+        <v>242</v>
       </c>
       <c r="D10" s="63"/>
-      <c r="E10" s="92"/>
+      <c r="E10" s="67"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2196,8 +2192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14433F0F-1925-450E-AF52-5B31D2F48EE0}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C21"/>
+    <sheetView topLeftCell="C14" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2243,56 +2239,56 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="81">
         <v>43369.583333333336</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="77"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="75"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="65"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -2302,8 +2298,8 @@
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -2313,59 +2309,59 @@
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="75"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="70"/>
+      <c r="C17" s="77"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="65"/>
+      <c r="C18" s="75"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="65"/>
+      <c r="C19" s="75"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="70"/>
+      <c r="C20" s="77"/>
     </row>
     <row r="21" spans="1:9" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="75" t="s">
-        <v>248</v>
-      </c>
-      <c r="C21" s="76"/>
+      <c r="B21" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="73"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
@@ -2529,6 +2525,12 @@
     <protectedRange sqref="D14:G15" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="13">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -2536,12 +2538,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 C18" xr:uid="{A0D75A70-63F2-4ABB-881B-C35F2C3A24A7}">
@@ -2558,10 +2554,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{160B54CD-E171-41D3-80E3-3CEE2B1A23A3}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A4" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2603,7 +2599,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2611,7 +2607,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2623,56 +2619,56 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="82">
+      <c r="B12" s="83">
         <v>43370.390277777777</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="84"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="75"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="65"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -2682,8 +2678,8 @@
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -2693,104 +2689,104 @@
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="75"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="86"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="65"/>
+      <c r="C18" s="75"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="87" t="s">
         <v>197</v>
       </c>
-      <c r="C20" s="79"/>
+      <c r="C20" s="87"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
-      <c r="B21" s="80" t="s">
+      <c r="B21" s="88" t="s">
         <v>198</v>
       </c>
-      <c r="C21" s="81"/>
+      <c r="C21" s="89"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="88" t="s">
         <v>200</v>
       </c>
-      <c r="C22" s="81"/>
+      <c r="C22" s="89"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="80" t="s">
-        <v>204</v>
-      </c>
-      <c r="C23" s="81"/>
+      <c r="B23" s="88" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="89"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
-      <c r="B24" s="80" t="s">
-        <v>211</v>
-      </c>
-      <c r="C24" s="81"/>
+      <c r="B24" s="88" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="89"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
-      <c r="B25" s="80" t="s">
-        <v>210</v>
-      </c>
-      <c r="C25" s="81"/>
+      <c r="B25" s="88" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" s="89"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
-      <c r="B26" s="80" t="s">
-        <v>213</v>
-      </c>
-      <c r="C26" s="81"/>
+      <c r="B26" s="88" t="s">
+        <v>210</v>
+      </c>
+      <c r="C26" s="89"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
-      <c r="B27" s="80" t="s">
-        <v>212</v>
-      </c>
-      <c r="C27" s="81"/>
+      <c r="B27" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="C27" s="89"/>
     </row>
     <row r="28" spans="1:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="75" t="s">
-        <v>214</v>
-      </c>
-      <c r="C28" s="76"/>
+      <c r="B28" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" s="73"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
@@ -2866,7 +2862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <v>2</v>
       </c>
@@ -2907,7 +2903,7 @@
       </c>
       <c r="O33" s="53"/>
     </row>
-    <row r="34" spans="1:15" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>3</v>
       </c>
@@ -2944,11 +2940,14 @@
         <v>85</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="O34" s="57"/>
-    </row>
-    <row r="35" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+      <c r="O34" s="30"/>
+      <c r="P34" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="45" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
         <v>4</v>
       </c>
@@ -2987,11 +2986,11 @@
         <v>88</v>
       </c>
       <c r="N35" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O35" s="30"/>
     </row>
-    <row r="36" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" ht="45" x14ac:dyDescent="0.2">
       <c r="A36" s="14">
         <v>5</v>
       </c>
@@ -3030,11 +3029,14 @@
         <v>88</v>
       </c>
       <c r="N36" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O36" s="57"/>
-    </row>
-    <row r="37" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="P36" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
@@ -3067,11 +3069,11 @@
         <v>91</v>
       </c>
       <c r="N37" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O37" s="57"/>
     </row>
-    <row r="38" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -3104,11 +3106,11 @@
         <v>91</v>
       </c>
       <c r="N38" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O38" s="57"/>
     </row>
-    <row r="39" spans="1:15" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -3141,11 +3143,11 @@
         <v>94</v>
       </c>
       <c r="N39" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O39" s="57"/>
     </row>
-    <row r="40" spans="1:15" ht="101.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -3178,11 +3180,11 @@
         <v>95</v>
       </c>
       <c r="N40" s="11" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="O40" s="57"/>
     </row>
-    <row r="41" spans="1:15" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -3215,11 +3217,11 @@
         <v>80</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O41" s="30"/>
     </row>
-    <row r="42" spans="1:15" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="11"/>
       <c r="C42" s="11"/>
@@ -3252,11 +3254,11 @@
         <v>80</v>
       </c>
       <c r="N42" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O42" s="30"/>
     </row>
-    <row r="43" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -3289,11 +3291,11 @@
         <v>88</v>
       </c>
       <c r="N43" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O43" s="30"/>
     </row>
-    <row r="44" spans="1:15" ht="101.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -3326,11 +3328,11 @@
         <v>80</v>
       </c>
       <c r="N44" s="11" t="s">
-        <v>208</v>
+        <v>249</v>
       </c>
       <c r="O44" s="57"/>
     </row>
-    <row r="45" spans="1:15" ht="101.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -3363,25 +3365,25 @@
         <v>98</v>
       </c>
       <c r="N45" s="15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="O45" s="58"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
       <c r="D46" s="37"/>
       <c r="E46" s="37"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
       <c r="D47" s="37"/>
       <c r="E47" s="37"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -3410,12 +3412,6 @@
     <protectedRange sqref="D14:G15" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="20">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -3430,6 +3426,12 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 C18" xr:uid="{B1942ADD-0981-4B08-9A53-0BFFD8BAE153}">
@@ -3448,8 +3450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875A633D-6CC0-49F3-94BF-53EB52B92CAE}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3506,56 +3508,56 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="81">
         <v>43370.559027777781</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="77"/>
     </row>
     <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="75"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="65"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -3565,10 +3567,10 @@
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="74" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="65"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -3578,53 +3580,53 @@
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="75"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="86"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="65"/>
+      <c r="C18" s="75"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="79"/>
+      <c r="C20" s="87"/>
     </row>
     <row r="21" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="76"/>
+      <c r="B21" s="72"/>
+      <c r="C21" s="73"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
@@ -3728,7 +3730,7 @@
         <v>116</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="N26" s="30"/>
     </row>
@@ -3766,7 +3768,7 @@
         <v>119</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="N27" s="30"/>
     </row>
@@ -3806,7 +3808,7 @@
         <v>119</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="N28" s="57"/>
     </row>
@@ -3846,7 +3848,7 @@
         <v>121</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="N29" s="57"/>
     </row>
@@ -3880,7 +3882,7 @@
         <v>122</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="N30" s="59"/>
     </row>
@@ -3914,7 +3916,7 @@
         <v>119</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -3948,7 +3950,7 @@
         <v>119</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="N32" s="59"/>
     </row>
@@ -3982,7 +3984,7 @@
         <v>121</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="N33" s="57"/>
     </row>
@@ -4016,7 +4018,7 @@
         <v>116</v>
       </c>
       <c r="M34" s="15" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="N34" s="60"/>
     </row>
@@ -4024,6 +4026,388 @@
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
+    </row>
+  </sheetData>
+  <protectedRanges>
+    <protectedRange sqref="D14:G15" name="Range1_2"/>
+  </protectedRanges>
+  <mergeCells count="13">
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18 B18:B19" xr:uid="{EE89E9F9-9BF4-4218-AE5E-3DF9B7CE52B9}">
+      <formula1>$F$1:$F$4</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{58496367-1F49-4E52-808E-C7C20D703DB6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC1C93F-1AD4-4CB6-934A-0B3A6BE1A849}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="3" width="35.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+    </row>
+    <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="80"/>
+    </row>
+    <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="75"/>
+    </row>
+    <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="92">
+        <v>43370.433333333334</v>
+      </c>
+      <c r="C12" s="75"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="75"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="75"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="75"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="75"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="85" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="86"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="75"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="87" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="87"/>
+    </row>
+    <row r="21" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="90"/>
+      <c r="C21" s="91"/>
+    </row>
+    <row r="24" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="24">
+        <v>1</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="47"/>
+      <c r="E25" s="53"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>2</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="30"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>3</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="30"/>
+    </row>
+    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10">
+        <v>4</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="30"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>5</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="30"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="10">
+        <v>6</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="10">
+        <v>7</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="30"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="10">
+        <v>8</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="37"/>
+      <c r="E32" s="30"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>9</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="30"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="14">
+        <v>10</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="48"/>
+      <c r="E34" s="33"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="2" t="s">
+        <v>218</v>
+      </c>
     </row>
   </sheetData>
   <protectedRanges>
@@ -4045,388 +4429,6 @@
     <mergeCell ref="B20:C20"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18 B18:B19" xr:uid="{EE89E9F9-9BF4-4218-AE5E-3DF9B7CE52B9}">
-      <formula1>$F$1:$F$4</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{58496367-1F49-4E52-808E-C7C20D703DB6}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DC1C93F-1AD4-4CB6-934A-0B3A6BE1A849}">
-  <dimension ref="A1:G42"/>
-  <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="3" width="35.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-    </row>
-    <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="67" t="s">
-        <v>107</v>
-      </c>
-      <c r="C10" s="68"/>
-    </row>
-    <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="65"/>
-    </row>
-    <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="84">
-        <v>43370.433333333334</v>
-      </c>
-      <c r="C12" s="65"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="65"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="64" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="65"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="65"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="77" t="s">
-        <v>223</v>
-      </c>
-      <c r="C17" s="78"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="64" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="65"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="79" t="s">
-        <v>222</v>
-      </c>
-      <c r="C20" s="79"/>
-    </row>
-    <row r="21" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="73"/>
-    </row>
-    <row r="24" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="24">
-        <v>1</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="47"/>
-      <c r="E25" s="53"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="10">
-        <v>2</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="30"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="10">
-        <v>3</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="30"/>
-    </row>
-    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
-        <v>4</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="30"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
-        <v>5</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="30"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
-        <v>6</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="30"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="10">
-        <v>7</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="30"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="10">
-        <v>8</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="30"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="10">
-        <v>9</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="30"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
-        <v>10</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="D34" s="48"/>
-      <c r="E34" s="33"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-  </sheetData>
-  <protectedRanges>
-    <protectedRange sqref="D14:G15" name="Range1_2"/>
-  </protectedRanges>
-  <mergeCells count="13">
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-  </mergeCells>
-  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 C18" xr:uid="{BEEBD12A-5441-471D-8267-1BCDDFF1AB5F}">
       <formula1>$F$1:$F$4</formula1>
     </dataValidation>
@@ -4441,7 +4443,7 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C21"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -4492,54 +4494,54 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="81">
         <v>43370.582638888889</v>
       </c>
-      <c r="C12" s="70"/>
+      <c r="C12" s="77"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="75"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -4549,10 +4551,10 @@
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64" t="s">
-        <v>236</v>
-      </c>
-      <c r="C15" s="65"/>
+      <c r="B15" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" s="75"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -4562,55 +4564,55 @@
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="75"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="86"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="65"/>
+      <c r="C18" s="75"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="65"/>
+      <c r="C20" s="75"/>
     </row>
     <row r="21" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="75" t="s">
-        <v>248</v>
-      </c>
-      <c r="C21" s="76"/>
+      <c r="B21" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="73"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
@@ -4714,7 +4716,7 @@
         <v>150</v>
       </c>
       <c r="M26" s="11" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="N26" s="30"/>
     </row>
@@ -4752,7 +4754,7 @@
         <v>151</v>
       </c>
       <c r="M27" s="11" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="N27" s="30"/>
     </row>
@@ -4792,7 +4794,7 @@
         <v>153</v>
       </c>
       <c r="M28" s="11" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="N28" s="30"/>
     </row>
@@ -4826,7 +4828,7 @@
         <v>150</v>
       </c>
       <c r="M29" s="11" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="N29" s="30"/>
     </row>
@@ -4860,7 +4862,7 @@
         <v>154</v>
       </c>
       <c r="M30" s="11" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="N30" s="30"/>
     </row>
@@ -4894,7 +4896,7 @@
         <v>156</v>
       </c>
       <c r="M31" s="11" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="N31" s="30"/>
     </row>
@@ -4928,7 +4930,7 @@
         <v>157</v>
       </c>
       <c r="M32" s="11" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="N32" s="30"/>
     </row>
@@ -4962,7 +4964,7 @@
         <v>157</v>
       </c>
       <c r="M33" s="11" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="N33" s="30"/>
     </row>
@@ -4993,7 +4995,7 @@
         <v>159</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="N34" s="30"/>
     </row>
@@ -5023,7 +5025,7 @@
         <v>161</v>
       </c>
       <c r="M35" s="15" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="N35" s="61"/>
     </row>
@@ -5032,12 +5034,6 @@
     <protectedRange sqref="D14:G15" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="13">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -5045,6 +5041,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 C18" xr:uid="{30ADB8DD-FFAF-4CC5-B24A-B9ED444FF813}">
@@ -5063,8 +5065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650FB760-B5AE-4E8E-AA26-702C9D1B0054}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E25"/>
+    <sheetView topLeftCell="A6" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5090,14 +5092,14 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
@@ -5108,56 +5110,56 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="84">
+      <c r="B12" s="92">
         <v>43370.444444444445</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="75"/>
     </row>
     <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="75"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="64" t="s">
-        <v>224</v>
-      </c>
-      <c r="C14" s="65"/>
+      <c r="B14" s="74" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="75"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -5167,8 +5169,8 @@
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="65"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -5178,53 +5180,51 @@
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="75"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="86"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="65"/>
+      <c r="B18" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="75"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="79" t="s">
-        <v>225</v>
-      </c>
-      <c r="C20" s="79"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
     </row>
     <row r="21" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="73"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="91"/>
     </row>
     <row r="23" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
@@ -5236,7 +5236,7 @@
       <c r="C23" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="88" t="s">
+      <c r="D23" s="64" t="s">
         <v>28</v>
       </c>
       <c r="E23" s="62" t="s">
@@ -5251,7 +5251,7 @@
         <v>35</v>
       </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="89"/>
+      <c r="D24" s="65"/>
       <c r="E24" s="53"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -5267,7 +5267,7 @@
       <c r="D25" s="36"/>
       <c r="E25" s="30"/>
     </row>
-    <row r="26" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
         <v>3</v>
       </c>
@@ -5277,10 +5277,8 @@
       <c r="C26" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="D26" s="90" t="s">
-        <v>249</v>
-      </c>
-      <c r="E26" s="91"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="33"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
@@ -5302,12 +5300,6 @@
     <protectedRange sqref="D14:G15" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="13">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -5315,6 +5307,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 C18" xr:uid="{29D31F47-099E-491B-91B5-AE5E236A45F5}">
@@ -5376,54 +5374,54 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="84">
+      <c r="B12" s="92">
         <v>43370.4375</v>
       </c>
-      <c r="C12" s="65"/>
+      <c r="C12" s="75"/>
     </row>
     <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="75"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -5433,10 +5431,10 @@
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64" t="s">
-        <v>226</v>
-      </c>
-      <c r="C15" s="65"/>
+      <c r="B15" s="74" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="75"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -5446,53 +5444,53 @@
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="65"/>
+      <c r="C16" s="75"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="86"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="65"/>
+      <c r="C18" s="75"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="85"/>
-      <c r="C20" s="85"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
     </row>
     <row r="21" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="75" t="s">
-        <v>248</v>
-      </c>
-      <c r="C21" s="76"/>
+      <c r="B21" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="C21" s="73"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
@@ -5594,7 +5592,7 @@
         <v>176</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J26" s="30"/>
     </row>
@@ -5616,7 +5614,7 @@
         <v>177</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J27" s="30"/>
     </row>
@@ -5638,7 +5636,7 @@
         <v>179</v>
       </c>
       <c r="I28" s="10" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J28" s="33"/>
     </row>
@@ -5712,12 +5710,6 @@
     <protectedRange sqref="D14:G15" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="13">
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
@@ -5725,6 +5717,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 C18" xr:uid="{67D9BA0C-C89F-491E-91DF-8E402F8116B0}">
@@ -5743,8 +5741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6459D5DF-FC12-4046-955C-5EF0A28D7646}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5768,14 +5766,14 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
@@ -5786,54 +5784,54 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
     </row>
     <row r="10" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="79" t="s">
         <v>194</v>
       </c>
-      <c r="C10" s="68"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65"/>
+      <c r="C11" s="75"/>
     </row>
     <row r="12" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="86">
+      <c r="B12" s="94">
         <v>43370.416666666664</v>
       </c>
-      <c r="C12" s="87"/>
+      <c r="C12" s="95"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="82" t="s">
         <v>192</v>
       </c>
-      <c r="C13" s="65"/>
+      <c r="C13" s="75"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="65"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -5843,10 +5841,10 @@
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="65"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -5866,61 +5864,59 @@
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="86"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="65"/>
+      <c r="C18" s="75"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="65"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="85" t="s">
-        <v>227</v>
-      </c>
-      <c r="C20" s="85"/>
+      <c r="B20" s="93"/>
+      <c r="C20" s="93"/>
     </row>
     <row r="21" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="72"/>
-      <c r="C21" s="73"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="91"/>
     </row>
   </sheetData>
   <protectedRanges>
     <protectedRange sqref="D14:G15" name="Range1_2"/>
   </protectedRanges>
   <mergeCells count="12">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 C18" xr:uid="{AC7F70D2-3882-4832-BA21-BFE3000F8A8F}">

</xml_diff>